<commit_message>
fix: Revert to original working reading summarizer
</commit_message>
<xml_diff>
--- a/uploads/example_reading_summary.xlsx
+++ b/uploads/example_reading_summary.xlsx
@@ -458,15 +458,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Here's the data formatted for easy pasting into an Excel spreadsheet.  Livia would copy and paste this into a spreadsheet and save as example_reading_summary.xlsx
-**Name** | **Key Concepts &amp; Definitions** | **Relevance &amp; Curiosity**
-------- | -------- | --------
-Higher ed must get ahead of AI paradigm shift | *AI's impact on knowledge work:* AI tools like ChatGPT are rapidly automating tasks previously done by humans, impacting various industries, including higher education.  *Higher ed's respo...</t>
+          <t>| Name | Key concepts &amp; Definitions | Relevance &amp; Curiosity |</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Higher ed must get ahead of AI paradigm shift | *AI's impact on knowledge work:* AI tools like ChatGPT are rapidly automating tasks previously done by humans, impacting various industries, including higher education.  *Higher ed's response:*  Institutions are primarily focused on immediate concerns like academic integrity, instead of addressing larger issues of curriculum relevance and workforce preparation.  *The need for human-centric jobs:* The author argues that humans will always be needed for jobs requiring relationship-building and human interaction (teaching, social work, healthcare). *AI's impact on higher ed employment:* AI will automate many administrative and instructional tasks in higher ed, potentially displacing workers. *Rethinking education:* Education needs to focus on teaching students to work effectively with AI, not just to compete with it.  |  **Leveraging AI in Education:** The article directly addresses how AI is transforming higher ed, prompting discussion of its use in teaching, assessment, and administration.  **Career Readiness:** The article’s core message is about preparing students for a future dramatically altered by AI, making it very relevant to career readiness.  **Learning Design:** The article challenges traditional learning models and explores how education needs to adapt in response to AI.  I'm also curious about the author’s argument that there will still be a need for jobs requiring uniquely human skills like empathy and social interaction.  The part about needing more social workers and counselors in underperforming schools is also very relevant to me, even though it's not strictly AI-related.</t>
+          <t>| Higher ed must get ahead of AI paradigm shift (opinion) | AI is rapidly changing the nature of knowledge work, potentially displacing humans in many fields.  ChatGPT and similar AI tools can perform tasks previously requiring extensive human expertise (coding, writing). This raises concerns about workforce displacement and the need to rethink higher education's role in preparing students for the future. The article explores the need to shift from knowledge-based to competency-based education, focusing on what students *can do* rather than just what they know. | This is super relevant to my interest in leveraging AI in education. The article highlights the potential disruption of AI on the workforce, which connects to career readiness.  The discussion about competency-based education is directly related to learning design and its implications for K-12. The author's concern about the future of work also relates to soft skill development - what human skills will remain valuable in an AI-driven world? |</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: Add smart fallback from Gemini to demo mode on platform
</commit_message>
<xml_diff>
--- a/uploads/example_reading_summary.xlsx
+++ b/uploads/example_reading_summary.xlsx
@@ -453,20 +453,21 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>example_reading</t>
+          <t>The Future of AI in Education</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>• Higher ed must get ahead of AI paradigm shift (opinion)	* **AI's impact on the workforce:**  AI, specifically large language models like ChatGPT, is rapidly automating knowledge work, potentially displacing human workers in various fields.
-• * **Higher education's response:** Higher ed institutions are primarily focused on immediate concerns like academic integrity, rather than the broader implications of AI on the future of work and education.
-• * **Rethinking curricula:**  AI is rapidly making existing curricula obsolete; we need to focus on how to use AI as a tool and develop higher-order cognitive skills.</t>
+          <t>• Artificial Intelligence in Education (AIEd) - The use of AI technologies to enhance learning experiences
+• Personalized Learning - Tailoring educational content to individual student needs
+• Learning Analytics - The measurement and analysis of learning data to improve outcomes</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>• * **Edtechs:** The rise of AI-powered edtech tools is a huge development discussed, impacting both learning design and career readiness.
-• * **Learning Design:**  The article emphasizes the need to rethink learning design in light of AI, focusing on higher-order cognitive skills and preparing students for a changing job market.</t>
+          <t>• Directly relevant to Livia's interests in leveraging AI for educational equity
+• Connects to her work with marginalized communities and learning design
+• Provides insights into career readiness and K-12 education applications</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix Excel and platform display consistency
</commit_message>
<xml_diff>
--- a/uploads/example_reading_summary.xlsx
+++ b/uploads/example_reading_summary.xlsx
@@ -453,21 +453,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>The Future of AI in Education</t>
+          <t>We’re Asking the Wrong Questions About AI</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>• Artificial Intelligence in Education (AIEd) - The use of AI technologies to enhance learning experiences
-• Personalized Learning - Tailoring educational content to individual student needs
-• Learning Analytics - The measurement and analysis of learning data to improve outcomes</t>
+          <t>Okay, so this article is all about how AI is changing the game, especially for education and the workforce. Here's the gist:
+*   AI is coming for knowledge work jobs, like coding and maybe even curriculum design!
+*   We need to rethink what students need to know and *do* in a world where AI can do a lot of the basic cognitive stuff.
+*   Competency-based education might be the way to go, focusing on skills and application.
+*   There's a big opportunity to focus on uniquely human skills, like teaching, social work, and mental health support - jobs that AI can't really do.
+*   We need to value and pay those 'human' jobs more!</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>• Directly relevant to Livia's interests in leveraging AI for educational equity
-• Connects to her work with marginalized communities and learning design
-• Provides insights into career readiness and K-12 education applications</t>
+          <t>Girl, this is SO relevant to our interests! Think about it: AI in education is a huge topic, and this article talks about how it's impacting curriculum and job prospects. It also brings up the importance of soft skills, which is totally your thing. Plus, the focus on valuing human-centered jobs could be a game-changer for marginalized communities if we can create pathways into those fields. And of course, it touches on how edtech and learning design need to adapt to this new AI reality. Basically, it's hitting all the key points!</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Clean up content to show only bullet points
</commit_message>
<xml_diff>
--- a/uploads/example_reading_summary.xlsx
+++ b/uploads/example_reading_summary.xlsx
@@ -453,22 +453,29 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>We’re Asking the Wrong Questions About AI</t>
+          <t>Higher ed must get ahead of AI paradigm shift (opinion)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Okay, so this article is all about how AI is changing the game, especially for education and the workforce. Here's the gist:
-*   AI is coming for knowledge work jobs, like coding and maybe even curriculum design!
-*   We need to rethink what students need to know and *do* in a world where AI can do a lot of the basic cognitive stuff.
-*   Competency-based education might be the way to go, focusing on skills and application.
-*   There's a big opportunity to focus on uniquely human skills, like teaching, social work, and mental health support - jobs that AI can't really do.
-*   We need to value and pay those 'human' jobs more!</t>
+          <t>* AI is rapidly changing the definition of knowledge work and potentially displacing human workers.
+* Higher education needs to address the larger questions posed by AI, not just academic integrity.
+* Competency-based education models may become more relevant as AI handles basic cognitive tasks.
+* Curricula need to be updated to reflect the changing demands of the workforce in the age of AI.
+* Universities can leverage AI for administrative processes, instruction, and tutoring, but must also address potential job displacement.
+* Society needs to value and invest in distinctly human jobs that algorithms cannot do, such as teaching, social work, and mental health care.
+* Universities need philosophers, ethicists, historians, sociologists, psychologists, cognitive scientists, and law faculty to address the complexities of AI.
+* Interdisciplinary collaboration is crucial to understanding and managing the impact of AI.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Girl, this is SO relevant to our interests! Think about it: AI in education is a huge topic, and this article talks about how it's impacting curriculum and job prospects. It also brings up the importance of soft skills, which is totally your thing. Plus, the focus on valuing human-centered jobs could be a game-changer for marginalized communities if we can create pathways into those fields. And of course, it touches on how edtech and learning design need to adapt to this new AI reality. Basically, it's hitting all the key points!</t>
+          <t>* Addresses leveraging AI in education, specifically how AI tools are changing higher education and potentially K-12.
+* Discusses career readiness as AI changes the skills needed for the workforce.
+* Touches on the potential displacement of workers, which is relevant to career readiness and soft skill development.
+* Highlights the need for uniquely human skills, implicitly emphasizing soft skill development.
+* Examines the role of edtechs in instruction, tutoring and advising.
+* Raises important questions regarding learning design and how AI may change the role of knowledge in learning.</t>
         </is>
       </c>
     </row>

</xml_diff>